<commit_message>
fix xlsx for tests
</commit_message>
<xml_diff>
--- a/tests/sample2.xlsx
+++ b/tests/sample2.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27510"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yusuke.okada/GoogleDrive/projects/xlsxconverter/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yusuke.okada/GoogleDrive/projects/xlsxconverter/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -817,7 +817,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
         <v>54</v>
@@ -882,7 +882,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>60</v>
@@ -950,7 +950,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>65</v>

</xml_diff>